<commit_message>
I had error with y position of ch 32.
This bux has been fixed. Now I calc X and Y coordinates correctly using 3x5 and 5x3 channels.
</commit_message>
<xml_diff>
--- a/VS2013/Parser/CoG_test.xlsx
+++ b/VS2013/Parser/CoG_test.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repositories\Parser_signal_finder\VS2013\Parser\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24075" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -53,12 +58,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -73,8 +84,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -84,6 +96,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -132,7 +147,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -167,7 +182,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -379,7 +394,7 @@
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,13 +434,13 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G2">
         <v>10</v>
@@ -435,81 +450,81 @@
       </c>
       <c r="J2">
         <f>(-2*$G$2)*A2 + (-1*$G$2)*B2 + (0*$G$2)*C2 + (1*$G$2)*D2 + (2*$G$2)*E2</f>
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="K2">
         <f>SUM(A2:E2)</f>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M2">
         <f>(2*$H$2)*A2 + (1*$H$2)*A3 + (0*$H$2)*A4 + (-1*$H$2)*A5 + (-2*$H$2)*A6</f>
-        <v>-310</v>
+        <v>-190</v>
       </c>
       <c r="N2">
         <f>(2*$H$2)*B2 + (1*$H$2)*B3 + (0*$H$2)*B4 + (-1*$H$2)*B5 + (-2*$H$2)*B6</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="O2">
         <f>(2*$H$2)*C2 + (1*$H$2)*C3 + (0*$H$2)*C4 + (-1*$H$2)*C5 + (-2*$H$2)*C6</f>
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="R2">
         <f>SUM(J2:J4)/SUM(K2:K4)</f>
-        <v>-0.24691358024691357</v>
+        <v>-2.7586206896551726</v>
       </c>
       <c r="S2">
         <f>SUM(M2:O2)/SUM(M5:O5)</f>
-        <v>-2.7472527472527473</v>
+        <v>-0.92592592592592593</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
       <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
         <v>4</v>
-      </c>
-      <c r="D3">
-        <v>8</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
       </c>
       <c r="J3">
         <f>(-2*$G$2)*A3 + (-1*$G$2)*B3 + (0*$G$2)*C3 + (1*$G$2)*D3 + (2*$G$2)*E3</f>
-        <v>30</v>
+        <v>-100</v>
       </c>
       <c r="K3">
         <f t="shared" ref="K3:K4" si="0">SUM(A3:E3)</f>
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C4">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J4">
         <f>(-2*$G$2)*A4 + (-1*$G$2)*B4 + (0*$G$2)*C4 + (1*$G$2)*D4 + (2*$G$2)*E4</f>
-        <v>-170</v>
+        <v>-210</v>
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M4" t="s">
         <v>6</v>
@@ -517,33 +532,36 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
         <v>4</v>
       </c>
-      <c r="C5">
-        <v>3</v>
+      <c r="D5" s="1">
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="M5">
         <f>SUM(A2:A6)</f>
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="N5">
         <f>SUM(B2:B6)</f>
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="O5">
         <f>SUM(C2:C6)</f>
-        <v>30</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>6</v>
@@ -552,7 +570,10 @@
         <v>7</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Different code for SiPM and PMT/GEM has been added
</commit_message>
<xml_diff>
--- a/VS2013/Parser/CoG_test.xlsx
+++ b/VS2013/Parser/CoG_test.xlsx
@@ -394,7 +394,7 @@
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,7 +470,7 @@
       </c>
       <c r="R2">
         <f>SUM(J2:J4)/SUM(K2:K4)</f>
-        <v>-2.7586206896551726</v>
+        <v>-0.69306930693069302</v>
       </c>
       <c r="S2">
         <f>SUM(M2:O2)/SUM(M5:O5)</f>
@@ -513,18 +513,18 @@
         <v>14</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J4">
         <f>(-2*$G$2)*A4 + (-1*$G$2)*B4 + (0*$G$2)*C4 + (1*$G$2)*D4 + (2*$G$2)*E4</f>
-        <v>-210</v>
+        <v>-40</v>
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="M4" t="s">
         <v>6</v>
@@ -544,7 +544,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="M5">
         <f>SUM(A2:A6)</f>
@@ -570,7 +570,7 @@
         <v>7</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E6" s="1">
         <v>0</v>

</xml_diff>